<commit_message>
lan cuoi (di ben em thay xot xa nguoi oi)
</commit_message>
<xml_diff>
--- a/phan_2/data/data_gdtx.xlsx
+++ b/phan_2/data/data_gdtx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\it004\da1\phan_2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2757D43-E543-40F2-8725-DB1CC7033D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBCCC66-8320-458A-92B2-03E097BC760E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1044,7 +1044,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>